<commit_message>
Check lại test Login
</commit_message>
<xml_diff>
--- a/PT_Docs/PT_Login.xlsx
+++ b/PT_Docs/PT_Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Tai Lieu_Talent\PT_Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Talent\TalentTechDocs\PT_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C540ED9-BEFB-4F3A-8709-07A6C3CAE3D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89B5123-1250-4C87-80FD-FC249D5FFC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="109">
   <si>
     <t>TC_01</t>
   </si>
@@ -118,10 +118,6 @@
 - Không có lỗi</t>
   </si>
   <si>
-    <t>- Ngừng xử lý
-- Message : "Định dạng email không chính xác"</t>
-  </si>
-  <si>
     <t>Hiển Thị Ban Đầu</t>
   </si>
   <si>
@@ -160,9 +156,6 @@
   </si>
   <si>
     <t>TC_24</t>
-  </si>
-  <si>
-    <t>TC_25</t>
   </si>
   <si>
     <t>Đúng format abc@gmail.com</t>
@@ -230,9 +223,6 @@
     <t>Quên mật khẩu</t>
   </si>
   <si>
-    <t>Di chuyển đến trang Quên mật khẩu</t>
-  </si>
-  <si>
     <t>Password có dấu</t>
   </si>
   <si>
@@ -268,12 +258,6 @@
     <t>Di chuyển đến Page Đăng ký tài khoản mới</t>
   </si>
   <si>
-    <t>Đăng nhập Account Google thành công</t>
-  </si>
-  <si>
-    <t>Thời điểm login sẽ được cập nhật trong DB</t>
-  </si>
-  <si>
     <t>Nhập email/Tài khoản không tồn tại</t>
   </si>
   <si>
@@ -307,12 +291,6 @@
   </si>
   <si>
     <t>Sai</t>
-  </si>
-  <si>
-    <t>email_verified_at</t>
-  </si>
-  <si>
-    <t>Được gửi về trong thời điểm Login</t>
   </si>
   <si>
     <t>Button Đăng nhập</t>
@@ -326,14 +304,6 @@
     <t>Link nhớ mật khẩu</t>
   </si>
   <si>
-    <t>Trạng thái: Uncheck
-Tài khoản sẽ tự động logout nếu trang web tắt</t>
-  </si>
-  <si>
-    <t>Trạng thái: Check
-Tài khoản vẫn được giữ nguyên nếu trang web tắt</t>
-  </si>
-  <si>
     <t>TC_27</t>
   </si>
   <si>
@@ -343,9 +313,6 @@
     <t>TC_29</t>
   </si>
   <si>
-    <t>TC_30</t>
-  </si>
-  <si>
     <t>TC_31</t>
   </si>
   <si>
@@ -362,9 +329,6 @@
   </si>
   <si>
     <t>Message : "Hãy nhập Email của bạn"</t>
-  </si>
-  <si>
-    <t>Message : "Hãy nhập Mật khẩu của bạn"</t>
   </si>
   <si>
     <t>Message khác tài liệu</t>
@@ -377,7 +341,34 @@
 Lưu ý : không viết testcase tài liệu không ghi, nếu e thấy cần thiết cái j đó thì nói a sửa tài liệu, r e dựa theo tài liệu mới để thêm testcase mới . ^^</t>
   </si>
   <si>
-    <t>Testcase này không cần, framework đang sử dụng support chuyện này r</t>
+    <t>Di chuyển đến Page Quên mật khẩu</t>
+  </si>
+  <si>
+    <t>Uncheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Tài khoản sẽ tự động logout sau 120p không hoạt động</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Tài khoản vẫn được giữ nguyên nếu trang web tắt</t>
+  </si>
+  <si>
+    <t>Email trong bảng User</t>
+  </si>
+  <si>
+    <t>name trong bảng User</t>
+  </si>
+  <si>
+    <t>Được lưu về bảng Users</t>
+  </si>
+  <si>
+    <t>- Ngừng xử lý
+- Message : "Email đã nhập không khớp với bất kỳ tài khoản nào! "</t>
+  </si>
+  <si>
+    <t>Message : "Hãy nhập Mật khẩu "</t>
   </si>
 </sst>
 </file>
@@ -502,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -552,17 +543,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -573,34 +573,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,476 +601,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>67234</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>123266</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>537882</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Speech Bubble: Rectangle 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32D5201-CADD-4B46-BB26-766893235478}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="997322" y="8516472"/>
-          <a:ext cx="1770531" cy="2106706"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Vùng</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> này là " Xử lý đăng ký "</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> Và đối tượng test là gì ? sao bỏ trống </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>- Nếu e đã mô tả IdHash,.. thì tại sao không mô tả cả name, email , ... theo tài liệu có gghi</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2566147</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>4336678</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>235324</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Speech Bubble: Rectangle 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF06F3D2-50D6-4F9F-B207-BC9134C453DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9480176" y="10130118"/>
-          <a:ext cx="1770531" cy="1109382"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>câu</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> này tối nghĩa, a có mô tả trong tài liệu là " thời điểm login " kìa</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1497106</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>62753</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3267637</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Speech Bubble: Rectangle 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21AAFA2C-EFCA-46E8-A7B9-054711698435}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5116606" y="9173135"/>
-          <a:ext cx="1770531" cy="1109382"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>nội</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> dung này nên nằm ở cột kết quả mong muốn</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>96370</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>342901</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>51548</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>85165</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Speech Bubble: Rectangle 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0215C4FA-C3D9-4455-A0A3-161C72D65F42}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12209929" y="10966077"/>
-          <a:ext cx="1770531" cy="1109382"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -210706"/>
-            <a:gd name="adj2" fmla="val 14015"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Page và</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> trang </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>nên</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> thống nhất 1 loại , 1 là dùng Page, 2 là dùng trang</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1154205</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2924736</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>56029</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Speech Bubble: Rectangle 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{794AFA3B-A376-4656-B9CA-68CDA61D8DCB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4773705" y="13749618"/>
-          <a:ext cx="1770531" cy="1109382"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 15243"/>
-            <a:gd name="adj2" fmla="val -109217"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Trạng</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> thái Uncheck , Check phải nằm trong cột này chứ nhỉ, sao lại nằm ở cột kết quả mong muốn.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>829234</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100851</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>235323</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>145675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Speech Bubble: Rectangle 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF39FD66-828A-4EDB-A710-57768BA67153}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12113558" y="13671175"/>
-          <a:ext cx="1445559" cy="1277471"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -163419"/>
-            <a:gd name="adj2" fmla="val -117564"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Tài</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> khoản sẽ tự logout sau 120p không hoạt động</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>A đã bô sung vvào tài liệu</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1353,23 +868,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="65.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="6"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="19.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="65.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="6"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
@@ -1392,142 +907,142 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="23" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="16"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="17"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>31</v>
+      <c r="B6" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="23" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>29</v>
@@ -1535,14 +1050,14 @@
       <c r="F11" s="8"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>27</v>
@@ -1550,14 +1065,14 @@
       <c r="F12" s="8"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>29</v>
@@ -1565,14 +1080,14 @@
       <c r="F13" s="8"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>29</v>
@@ -1580,32 +1095,32 @@
       <c r="F14" s="8"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>107</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="5"/>
-      <c r="I15" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>29</v>
@@ -1613,353 +1128,348 @@
       <c r="F16" s="8"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="5"/>
-      <c r="I17" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="15" t="s">
-        <v>34</v>
+      <c r="B18" s="21"/>
+      <c r="C18" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>107</v>
+        <v>52</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="5"/>
-      <c r="I18" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I18" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="5"/>
       <c r="I19" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
+        <v>36</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+        <v>37</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
+        <v>38</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
+        <v>39</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>56</v>
+        <v>40</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="19"/>
+        <v>41</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="19"/>
+        <v>42</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>78</v>
+        <v>51</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="5"/>
-      <c r="I27" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="2" t="s">
-        <v>61</v>
+        <v>88</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="20" t="s">
+        <v>81</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="12" t="s">
         <v>89</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>73</v>
+        <v>90</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>84</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F31" s="8"/>
+    <row r="31" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="14"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="14"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="14"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="14"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="31" t="s">
         <v>100</v>
-      </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="32" t="s">
-        <v>65</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="8"/>
+        <v>92</v>
+      </c>
+      <c r="B34" s="22"/>
+      <c r="C34" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="D34" s="2"/>
-      <c r="E34" s="32" t="s">
-        <v>76</v>
+      <c r="E34" s="31" t="s">
+        <v>73</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="27" t="s">
-        <v>95</v>
+      <c r="B36" s="21"/>
+      <c r="C36" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C24:C30"/>
+    <mergeCell ref="B24:B34"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C18:C23"/>
     <mergeCell ref="B9:B23"/>
     <mergeCell ref="C9:C17"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="B24:B28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Login test Doc ( 2)
</commit_message>
<xml_diff>
--- a/PT_Docs/PT_Login.xlsx
+++ b/PT_Docs/PT_Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Talent\TalentTechDocs\PT_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5325414-17AD-4418-861D-0AB6EEBED1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A0AB3D-CD5D-426C-8202-212A6F480AF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="105">
   <si>
     <t>TC_01</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>TC_07</t>
+  </si>
+  <si>
+    <t>TC_08</t>
   </si>
   <si>
     <t>TC_09</t>
@@ -278,19 +281,16 @@
     <t>TC_27</t>
   </si>
   <si>
+    <t>TC_28</t>
+  </si>
+  <si>
+    <t>TC_29</t>
+  </si>
+  <si>
     <t>TC_31</t>
   </si>
   <si>
     <t>TC_32</t>
-  </si>
-  <si>
-    <t>TC_33</t>
-  </si>
-  <si>
-    <t>TC_34</t>
-  </si>
-  <si>
-    <t>TC_35</t>
   </si>
   <si>
     <t>Message : "Hãy nhập Email của bạn"</t>
@@ -343,10 +343,19 @@
     <t>idHash</t>
   </si>
   <si>
-    <t>db.users=users.name</t>
-  </si>
-  <si>
     <t>Duy trì đăng nhập</t>
+  </si>
+  <si>
+    <t>TC_25</t>
+  </si>
+  <si>
+    <t>TC_30</t>
+  </si>
+  <si>
+    <t>db.users= email trong cột email của bảng users</t>
+  </si>
+  <si>
+    <t>db.users=name trong cột name của bảng users</t>
   </si>
 </sst>
 </file>
@@ -465,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -520,6 +529,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -843,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -861,133 +873,133 @@
   <sheetData>
     <row r="2" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="23" t="s">
-        <v>22</v>
+      <c r="B3" s="27"/>
+      <c r="C3" s="24" t="s">
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="25"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>29</v>
+      <c r="B6" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="24" t="s">
         <v>24</v>
       </c>
+      <c r="C9" s="24" t="s">
+        <v>25</v>
+      </c>
       <c r="D9" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>85</v>
@@ -996,75 +1008,75 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>95</v>
       </c>
       <c r="F14" s="8"/>
@@ -1074,31 +1086,31 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="29" t="s">
         <v>73</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>74</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="5"/>
@@ -1107,17 +1119,17 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="23" t="s">
-        <v>32</v>
+      <c r="B17" s="25"/>
+      <c r="C17" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>96</v>
       </c>
       <c r="F17" s="8"/>
@@ -1127,15 +1139,15 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="31" t="s">
         <v>97</v>
       </c>
       <c r="F18" s="8"/>
@@ -1145,222 +1157,226 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="A19" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="23" t="s">
+      <c r="B23" s="24" t="s">
         <v>53</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="A26" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="A27" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="32" t="s">
         <v>98</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
-      <c r="B28" s="24"/>
+      <c r="A28" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="25"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="32" t="s">
-        <v>100</v>
+      <c r="E28" s="33" t="s">
+        <v>103</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
-      <c r="B29" s="24"/>
+      <c r="A29" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="25"/>
       <c r="C29" s="16"/>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E29" s="32" t="s">
-        <v>100</v>
+      <c r="E29" s="33" t="s">
+        <v>104</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="24"/>
+      <c r="A30" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="25"/>
       <c r="C30" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="22" t="s">
         <v>89</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="25"/>
+      <c r="A31" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="26"/>
       <c r="C31" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="21" t="s">
-        <v>71</v>
+      <c r="E31" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>77</v>
+      <c r="A32" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>78</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="22" t="s">
-        <v>101</v>
+      <c r="B33" s="25"/>
+      <c r="C33" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>90</v>
@@ -1372,13 +1388,13 @@
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="22"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Bao cao tien do lam test Users Mobile
</commit_message>
<xml_diff>
--- a/PT_Docs/PT_Login.xlsx
+++ b/PT_Docs/PT_Login.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Talent\TalentTechDocs\PT_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251C9405-7129-4A1B-B7F9-B18C08BA1035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EFD94-9F67-445B-8A5A-3CBB088090F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,10 +376,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Tài khoản bị Logout không hiện 
-thông báo</t>
-  </si>
-  <si>
     <t>(Cái này để tối em xác minh nha :v,)</t>
   </si>
   <si>
@@ -391,6 +387,10 @@
   </si>
   <si>
     <t>( Chưa có tài liệu của Tablet)</t>
+  </si>
+  <si>
+    <t>Tài khoản bị Logout không hiện 
+thông báo ( Giữa điện thoại - Microsoft Edge)</t>
   </si>
 </sst>
 </file>
@@ -603,23 +603,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -636,6 +621,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -651,8 +642,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,8 +979,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="44" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -998,8 +998,8 @@
       <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
@@ -1008,15 +1008,15 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1025,14 +1025,14 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="37" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -1051,7 +1051,7 @@
       <c r="A7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="11" t="s">
         <v>29</v>
       </c>
@@ -1068,7 +1068,7 @@
       <c r="A8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="33"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="11" t="s">
         <v>31</v>
       </c>
@@ -1085,10 +1085,10 @@
       <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -1106,8 +1106,8 @@
       <c r="A10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="23" t="s">
         <v>66</v>
       </c>
@@ -1121,8 +1121,8 @@
       <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="9" t="s">
         <v>96</v>
       </c>
@@ -1138,8 +1138,8 @@
       <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="9" t="s">
         <v>40</v>
       </c>
@@ -1156,8 +1156,8 @@
       <c r="A13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="9" t="s">
         <v>39</v>
       </c>
@@ -1173,8 +1173,8 @@
       <c r="A14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="9" t="s">
         <v>63</v>
       </c>
@@ -1191,8 +1191,8 @@
       <c r="A15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="44" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -1211,8 +1211,8 @@
       <c r="A16" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="23" t="s">
         <v>53</v>
       </c>
@@ -1226,8 +1226,8 @@
       <c r="A17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="9" t="s">
         <v>54</v>
       </c>
@@ -1243,8 +1243,8 @@
       <c r="A18" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="9" t="s">
         <v>56</v>
       </c>
@@ -1260,8 +1260,8 @@
       <c r="A19" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="9" t="s">
         <v>57</v>
       </c>
@@ -1277,8 +1277,8 @@
       <c r="A20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="9" t="s">
         <v>58</v>
       </c>
@@ -1294,10 +1294,10 @@
       <c r="A21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="36" t="s">
         <v>81</v>
       </c>
       <c r="D21" s="5"/>
@@ -1313,8 +1313,8 @@
       <c r="A22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="9" t="s">
         <v>51</v>
       </c>
@@ -1330,8 +1330,8 @@
       <c r="A23" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="9" t="s">
         <v>47</v>
       </c>
@@ -1347,8 +1347,8 @@
       <c r="A24" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="43"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="2" t="s">
         <v>49</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="31" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1364,11 +1364,11 @@
       <c r="A25" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="42" t="s">
+      <c r="B25" s="42"/>
+      <c r="C25" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="32" t="s">
         <v>84</v>
       </c>
       <c r="E25" s="26" t="s">
@@ -1383,9 +1383,9 @@
       <c r="A26" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="38"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="27" t="s">
         <v>91</v>
       </c>
@@ -1398,9 +1398,9 @@
       <c r="A27" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="39"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="27" t="s">
         <v>92</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="A28" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="39" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -1432,7 +1432,7 @@
       <c r="A29" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="43"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="13" t="s">
         <v>61</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="A30" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="36" t="s">
         <v>89</v>
       </c>
       <c r="C30" s="18" t="s">
@@ -1462,16 +1462,16 @@
       <c r="F30" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="47" t="s">
-        <v>103</v>
+      <c r="G30" s="31" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="40" t="s">
+      <c r="B31" s="37"/>
+      <c r="C31" s="35" t="s">
         <v>87</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -1482,15 +1482,15 @@
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="40"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="2" t="s">
         <v>22</v>
       </c>
@@ -1498,12 +1498,17 @@
         <v>76</v>
       </c>
       <c r="F32" s="8"/>
-      <c r="G32" s="47" t="s">
-        <v>105</v>
+      <c r="G32" s="31" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="B9:B20"/>
+    <mergeCell ref="C9:C14"/>
     <mergeCell ref="D25:D27"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="B30:B32"/>
@@ -1512,11 +1517,6 @@
     <mergeCell ref="B21:B27"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="B9:B20"/>
-    <mergeCell ref="C9:C14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>